<commit_message>
Adding elements in Problem Page Problem test data is splitted Methods from Service Now Utils are moved
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="48" windowWidth="15156" windowHeight="7992"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="15150" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke_Suite" sheetId="3" r:id="rId1"/>
+    <sheet name="ProblemTask" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="AAN" comment="Change Model types present under the Subcategory AAN">#REF!</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
   <si>
     <t>Serial No.</t>
   </si>
@@ -84,21 +85,6 @@
     <t>Problem ID</t>
   </si>
   <si>
-    <t>Test Create Problem Ticket</t>
-  </si>
-  <si>
-    <t>Test Update Problem Ticket</t>
-  </si>
-  <si>
-    <t>Test Approve Problem Ticket</t>
-  </si>
-  <si>
-    <t>Test Close Problem Ticket</t>
-  </si>
-  <si>
-    <t>Test Create Problem Task Ticket</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -132,16 +118,31 @@
     <t>Biradar Nagesh</t>
   </si>
   <si>
-    <t>PRB02001531</t>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>PRB02001589</t>
+  </si>
+  <si>
+    <t>TestCreateProblemTicket</t>
+  </si>
+  <si>
+    <t>TestUpdateProblemTicket</t>
+  </si>
+  <si>
+    <t>TestApproveProblemTicket</t>
+  </si>
+  <si>
+    <t>TestCloseProblemTicket</t>
+  </si>
+  <si>
+    <t>TestCreateProblemTaskTicket</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>PRB02001536</t>
-  </si>
-  <si>
-    <t>Passed</t>
+    <t>PRB02001599</t>
   </si>
 </sst>
 </file>
@@ -215,9 +216,6 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -229,14 +227,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,347 +536,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="8.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="22.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.21875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="6.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="6.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="18.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="32.33203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="16.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="22.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="10.33203125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="3" width="16.5546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="3" width="31.44140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="3" width="17.88671875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="3" width="8.5546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="3" width="32.33203125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="3" width="16.44140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="3" width="18.5546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="3" width="17.5546875" collapsed="true"/>
-    <col min="19" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="6.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="16.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="31.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="8.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
+    <col min="19" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="6" customFormat="1" ht="12">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="24">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="24">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="22.8">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="24">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="5" t="s">
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="24">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="22.8">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="22.8">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="22.8">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="22.8">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="5" t="s">
+      <c r="J6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
       <formula1>"1 - Extensive / Widespread, 2 - Significant / Large, 3 - Moderate / Limited"</formula1>
     </dataValidation>
@@ -887,14 +778,157 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
       <formula1>"Change Management, Continuous Service Improvement, Event Monitoring, External Customer, Internal User, Notification from Supplier, Proactive Checks, Problem Management"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N6">
-      <formula1>"1 - Critical, 2 - High, 3 - Medium, 4 - Minor, 5 - Low"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6 O2:O6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
       <formula1>"DEVELOP-QA-SERVICE-MANAGER,DEVELOP-QA-SERVICE-MANAGER-AG"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" style="5" width="23.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="24">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="24">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="24">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="24">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="24">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6">
+      <formula1>"DEVELOP-QA-SERVICE-MANAGER,DEVELOP-QA-SERVICE-MANAGER-AG"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6">
+      <formula1>"1 - Critical, 2 - High, 3 - Medium, 4 - Minor, 5 - Low"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified problemManagement.java, ProblemReusables.java, ProblemPage.java, Problem_Management_TestData.xlsx
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="15150" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="15156" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke_Suite" sheetId="3" r:id="rId1"/>
@@ -42,12 +42,12 @@
     <definedName name="Telecom" comment="Subcategories present under the Category Telecom">#REF!</definedName>
     <definedName name="Unsuccessful">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="37">
   <si>
     <t>Serial No.</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Problem Management</t>
   </si>
   <si>
-    <t>Imact</t>
-  </si>
-  <si>
     <t>Complexity</t>
   </si>
   <si>
@@ -121,28 +118,46 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>PRB02001589</t>
-  </si>
-  <si>
-    <t>TestCreateProblemTicket</t>
-  </si>
-  <si>
-    <t>TestUpdateProblemTicket</t>
-  </si>
-  <si>
-    <t>TestApproveProblemTicket</t>
-  </si>
-  <si>
     <t>TestCloseProblemTicket</t>
   </si>
   <si>
     <t>TestCreateProblemTaskTicket</t>
   </si>
   <si>
+    <t>2 - Significant / Large</t>
+  </si>
+  <si>
+    <t>2 - Medium</t>
+  </si>
+  <si>
+    <t>3 - Moderate / Limited</t>
+  </si>
+  <si>
+    <t>3 - Low</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>testDifferentPhasesOfProblemTicket</t>
+  </si>
+  <si>
+    <t>testUpdateProblemTicket</t>
+  </si>
+  <si>
+    <t>testCreateProblemTicket</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>PRB02001599</t>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>PRB02001662</t>
+  </si>
+  <si>
+    <t>Accepted</t>
   </si>
 </sst>
 </file>
@@ -213,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -233,9 +248,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,33 +551,33 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" activeCellId="3" sqref="C4 C3 C2 C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="6.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="28.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="6.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="32.33203125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="16.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="31.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="8.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
-    <col min="19" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="22.109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="16.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="31.44140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="17.88671875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="8.5546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="32.33203125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.44140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="18.5546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="17.5546875" collapsed="true"/>
+    <col min="19" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="12">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -591,10 +603,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>8</v>
@@ -603,19 +615,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="24">
+    <row r="2" spans="1:12" ht="22.8">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -627,10 +639,10 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -639,16 +651,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="24">
+    <row r="3" spans="1:12" ht="22.8">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
@@ -659,10 +675,10 @@
         <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>10</v>
@@ -671,16 +687,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="24">
+    <row r="4" spans="1:12" ht="22.8">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
@@ -691,11 +713,11 @@
         <v>9</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="K4" s="4" t="s">
         <v>10</v>
       </c>
@@ -703,12 +725,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="24">
+    <row r="5" spans="1:12" ht="22.8">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -723,11 +745,11 @@
         <v>9</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="K5" s="4" t="s">
         <v>10</v>
       </c>
@@ -735,12 +757,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="24">
+    <row r="6" spans="1:12" ht="22.8">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -755,10 +777,10 @@
         <v>9</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>10</v>
@@ -795,9 +817,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="23.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" style="5" width="23.85546875" collapsed="true"/>
+    <col min="1" max="16384" style="5" width="23.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -805,13 +827,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -820,18 +842,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24">
+    <row r="2" spans="1:6" ht="22.8">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
@@ -840,18 +862,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24">
+    <row r="3" spans="1:6" ht="22.8">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
@@ -860,18 +882,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24">
+    <row r="4" spans="1:6" ht="22.8">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
@@ -880,18 +902,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24">
+    <row r="5" spans="1:6" ht="22.8">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -900,18 +922,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24">
+    <row r="6" spans="1:6" ht="22.8">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Adding Problem Reusables and Problem Test data
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="48" windowWidth="15156" windowHeight="7992"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18750" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke_Suite" sheetId="3" r:id="rId1"/>
@@ -42,12 +42,12 @@
     <definedName name="Telecom" comment="Subcategories present under the Category Telecom">#REF!</definedName>
     <definedName name="Unsuccessful">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
   <si>
     <t>Serial No.</t>
   </si>
@@ -115,57 +115,102 @@
     <t>Biradar Nagesh</t>
   </si>
   <si>
+    <t>2 - Significant / Large</t>
+  </si>
+  <si>
+    <t>2 - Medium</t>
+  </si>
+  <si>
+    <t>3 - Moderate / Limited</t>
+  </si>
+  <si>
+    <t>3 - Low</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Workaround</t>
+  </si>
+  <si>
+    <t>Root cause category</t>
+  </si>
+  <si>
+    <t>Root cause subcategory</t>
+  </si>
+  <si>
+    <t>Change Failure</t>
+  </si>
+  <si>
+    <t>Inadequate Execution</t>
+  </si>
+  <si>
+    <t>Root cause detail</t>
+  </si>
+  <si>
+    <t>Root cause CI</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Root cause analysis complete</t>
+  </si>
+  <si>
+    <t>Work notes</t>
+  </si>
+  <si>
+    <t>Test Create Problem Ticket</t>
+  </si>
+  <si>
+    <t>Test Update Problem Ticket</t>
+  </si>
+  <si>
+    <t>Test Different Phases Of ProblemTicket</t>
+  </si>
+  <si>
+    <t>Test Close Problem Ticket</t>
+  </si>
+  <si>
+    <t>Test Create Problem Task Ticket</t>
+  </si>
+  <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>TestCloseProblemTicket</t>
-  </si>
-  <si>
-    <t>TestCreateProblemTaskTicket</t>
-  </si>
-  <si>
-    <t>2 - Significant / Large</t>
-  </si>
-  <si>
-    <t>2 - Medium</t>
-  </si>
-  <si>
-    <t>3 - Moderate / Limited</t>
-  </si>
-  <si>
-    <t>3 - Low</t>
-  </si>
-  <si>
-    <t>Impact</t>
-  </si>
-  <si>
-    <t>testDifferentPhasesOfProblemTicket</t>
-  </si>
-  <si>
-    <t>testUpdateProblemTicket</t>
-  </si>
-  <si>
-    <t>testCreateProblemTicket</t>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Closed Complete</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>PRB02001733</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Work in Progress</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>PRB02001662</t>
-  </si>
-  <si>
-    <t>Accepted</t>
+    <t>PRB02001736</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -224,11 +269,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -247,8 +305,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,6 +403,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -372,6 +438,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -547,47 +614,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" activeCellId="3" sqref="C4 C3 C2 C3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="28.77734375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="6.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="32.33203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="6.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="16.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="22.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.33203125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="16.5546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="31.44140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="17.88671875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="8.5546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="32.33203125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.44140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="18.5546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="17.5546875" collapsed="true"/>
-    <col min="19" max="16384" style="2" width="9.109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="18.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="21.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="6.7109375" collapsed="true"/>
+    <col min="20" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -599,35 +667,56 @@
       <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>3</v>
+      <c r="P1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="22.8">
+    <row r="2" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -639,10 +728,10 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -650,20 +739,39 @@
       <c r="L2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="M2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="22.8">
+    <row r="3" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C3" s="10"/>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
@@ -675,10 +783,10 @@
         <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>10</v>
@@ -686,22 +794,43 @@
       <c r="L3" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="M3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="22.8">
+    <row r="4" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
@@ -724,17 +853,38 @@
       <c r="L4" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="M4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="22.8">
+    <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
@@ -756,17 +906,38 @@
       <c r="L5" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="M5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="22.8">
+    <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
@@ -788,9 +959,30 @@
       <c r="L6" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="M6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
       <formula1>"1 - Extensive / Widespread, 2 - Significant / Large, 3 - Moderate / Limited"</formula1>
     </dataValidation>
@@ -803,6 +995,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
       <formula1>"DEVELOP-QA-SERVICE-MANAGER,DEVELOP-QA-SERVICE-MANAGER-AG"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S6">
+      <formula1>"Work in Progress, Closed, Deferred"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -810,145 +1005,208 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="5" width="23.88671875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="16.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="7.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="13.5703125" collapsed="true"/>
+    <col min="6" max="8" bestFit="true" customWidth="true" style="5" width="21.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="5" width="23.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="22.8">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
+    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="22.8">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
+    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="22.8">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
+    <row r="4" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="22.8">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
+    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="22.8">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
+    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
       <formula1>"DEVELOP-QA-SERVICE-MANAGER,DEVELOP-QA-SERVICE-MANAGER-AG"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6">
       <formula1>"1 - Critical, 2 - High, 3 - Medium, 4 - Minor, 5 - Low"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
+      <formula1>"Open, Pending, Work in Progress, Closed Complete, Cancelled"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes made to ProblemReusables.java, ProblemTaskPage.java and its test data sheet
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Problem_Management_TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="21720" windowHeight="6375"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="21720" windowHeight="6372"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke_Suite" sheetId="3" r:id="rId1"/>
@@ -42,12 +42,12 @@
     <definedName name="Telecom" comment="Subcategories present under the Category Telecom">#REF!</definedName>
     <definedName name="Unsuccessful">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
   <si>
     <t>Serial No.</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Assigned to</t>
   </si>
   <si>
-    <t>Biradar Nagesh</t>
-  </si>
-  <si>
     <t>2 - Significant / Large</t>
   </si>
   <si>
@@ -169,12 +166,6 @@
     <t>Test Different Phases Of ProblemTicket</t>
   </si>
   <si>
-    <t>Test Close Problem Ticket</t>
-  </si>
-  <si>
-    <t>Test Create Problem Task Ticket</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
@@ -187,48 +178,42 @@
     <t>Closed</t>
   </si>
   <si>
-    <t>PRB02001745</t>
+    <t>PRB02001752</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>PRB02001668</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Sathyanarayanan V</t>
+  </si>
+  <si>
+    <t>PRB02001667</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>PRB02001746</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>PRB02001747</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>PRB02001748</t>
-  </si>
-  <si>
-    <t>PRB02001749</t>
-  </si>
-  <si>
-    <t>PRB02001750</t>
-  </si>
-  <si>
     <t>Work in Progress</t>
   </si>
   <si>
     <t>Known Error</t>
+  </si>
+  <si>
+    <t>PRB02003877</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,35 +235,19 @@
       <family val="2"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="9"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -300,6 +269,10 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color indexed="9"/>
     </font>
     <font>
@@ -309,6 +282,10 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color indexed="9"/>
     </font>
     <font>
@@ -386,7 +363,7 @@
       <color indexed="9"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,38 +377,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -444,83 +391,8 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -543,24 +415,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -584,41 +443,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +562,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -743,7 +596,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -919,38 +771,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="18.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="32.33203125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="16.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="22.109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="16.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="21.44140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="11.109375" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="18.0" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="6.7109375" collapsed="true"/>
-    <col min="20" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.44140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="12.109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="17.5546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="6.6640625" collapsed="true"/>
+    <col min="20" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="12">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -976,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>14</v>
@@ -988,40 +840,40 @@
         <v>3</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="P1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="S1" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="22.8">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" t="s" s="29">
-        <v>42</v>
+      <c r="E2" t="s" s="26">
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -1033,11 +885,11 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1048,10 +900,10 @@
         <v>10</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>10</v>
@@ -1060,23 +912,25 @@
         <v>9</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="22.8">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
       <c r="D3" s="3"/>
-      <c r="E3" t="s">
-        <v>42</v>
+      <c r="E3" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
@@ -1088,11 +942,11 @@
         <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="K3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1103,10 +957,10 @@
         <v>10</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>10</v>
@@ -1115,27 +969,27 @@
         <v>9</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="22.8">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s" s="38">
         <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s" s="41">
-        <v>42</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
@@ -1162,10 +1016,10 @@
         <v>10</v>
       </c>
       <c r="N4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>10</v>
@@ -1174,133 +1028,27 @@
         <v>9</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
       <formula1>"1 - Extensive / Widespread, 2 - Significant / Large, 3 - Moderate / Limited"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
       <formula1>"1 - High, 2 - Medium, 3 - Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
       <formula1>"Change Management, Continuous Service Improvement, Event Monitoring, External Customer, Internal User, Notification from Supplier, Proactive Checks, Problem Management"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
       <formula1>"DEVELOP-QA-SERVICE-MANAGER,DEVELOP-QA-SERVICE-MANAGER-AG"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S4">
       <formula1>"Work in Progress, Closed, Deferred"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1310,25 +1058,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E6" activeCellId="1" sqref="E2 E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="23.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="8.6640625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="16.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="7.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="13.5703125" collapsed="true"/>
-    <col min="6" max="8" bestFit="true" customWidth="true" style="5" width="21.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="5" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="7.109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="13.5546875" collapsed="true"/>
+    <col min="6" max="8" bestFit="true" customWidth="true" style="5" width="21.44140625" collapsed="true"/>
+    <col min="9" max="16384" style="5" width="23.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1351,13 +1099,13 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="22.8">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1371,7 +1119,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
@@ -1383,134 +1131,18 @@
         <v>10</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"DEVELOP-QA-SERVICE-MANAGER,DEVELOP-QA-SERVICE-MANAGER-AG"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"1 - Critical, 2 - High, 3 - Medium, 4 - Minor, 5 - Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
       <formula1>"Open, Pending, Work in Progress, Closed Complete, Cancelled"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>